<commit_message>
Fix issues for merge
</commit_message>
<xml_diff>
--- a/static_files/labelling_file.xlsx
+++ b/static_files/labelling_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\no-code-app\static_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive - IRESSEF\Documents\DSWB\Project\Training\Workshop_2025\Github\workshop_github\no-code-app\static_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86196AAE-E5DA-4440-860A-E6B3C06E070B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06E7E23-1B88-474A-B963-848390CD1D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43208FD5-7BAA-4932-9269-4D84D13319F6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{43208FD5-7BAA-4932-9269-4D84D13319F6}"/>
   </bookViews>
   <sheets>
     <sheet name="ui_labels" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="336">
   <si>
     <t>upload_file_local</t>
   </si>
@@ -1042,14 +1042,31 @@
   </si>
   <si>
     <t>Connexion à la base de données réussie</t>
+  </si>
+  <si>
+    <t>automl_title</t>
+  </si>
+  <si>
+    <t>Automl with Pycaret</t>
+  </si>
+  <si>
+    <t>Automl avec Pycaret</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1065,7 +1082,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1073,13 +1090,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1100,7 +1138,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1396,30 +1434,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C65CCAF-013C-4E8E-8632-543B46C7B55A}">
-  <dimension ref="A1:CN3"/>
+  <dimension ref="A1:CO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
-      <selection activeCell="CR2" sqref="CR2"/>
+    <sheetView tabSelected="1" topLeftCell="BX3" workbookViewId="0">
+      <selection activeCell="CO3" sqref="CO3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.61328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.07421875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.23046875" style="1"/>
-    <col min="5" max="5" width="47.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" style="1"/>
+    <col min="5" max="5" width="47.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.23046875" style="1"/>
-    <col min="9" max="9" width="19.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="77" width="9.23046875" style="1"/>
-    <col min="78" max="78" width="9.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="79" max="16384" width="9.23046875" style="1"/>
+    <col min="8" max="8" width="9.26953125" style="1"/>
+    <col min="9" max="9" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="77" width="9.26953125" style="1"/>
+    <col min="78" max="78" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="79" max="16384" width="9.26953125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" ht="102" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:93" ht="102" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1696,8 +1734,11 @@
       <c r="CN1" s="1" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="2" spans="1:92" ht="204" x14ac:dyDescent="0.4">
+      <c r="CO1" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:93" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1974,8 +2015,11 @@
       <c r="CN2" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="3" spans="1:92" ht="247.75" x14ac:dyDescent="0.4">
+      <c r="CO2" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:93" ht="247" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2251,6 +2295,9 @@
       </c>
       <c r="CN3" s="1" t="s">
         <v>332</v>
+      </c>
+      <c r="CO3" s="2" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -2266,15 +2313,15 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2288,7 +2335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2302,7 +2349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2316,7 +2363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2330,7 +2377,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2344,7 +2391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -2358,7 +2405,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -2372,7 +2419,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -2386,7 +2433,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -2403,7 +2450,7 @@
         <v>---Sélectionner le genre---</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -2417,7 +2464,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>177</v>
       </c>
@@ -2431,7 +2478,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -2445,7 +2492,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>229</v>
       </c>
@@ -2459,7 +2506,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -2473,7 +2520,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>229</v>
       </c>
@@ -2487,7 +2534,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>229</v>
       </c>
@@ -2501,7 +2548,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>232</v>
       </c>
@@ -2515,7 +2562,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>232</v>
       </c>
@@ -2529,7 +2576,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>237</v>
       </c>
@@ -2543,7 +2590,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>237</v>
       </c>
@@ -2557,7 +2604,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>256</v>
       </c>
@@ -2571,7 +2618,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>256</v>
       </c>
@@ -2585,7 +2632,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>256</v>
       </c>
@@ -2599,7 +2646,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>285</v>
       </c>
@@ -2613,7 +2660,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>285</v>
       </c>
@@ -2627,7 +2674,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>285</v>
       </c>
@@ -2641,7 +2688,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>302</v>
       </c>
@@ -2655,7 +2702,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>302</v>
       </c>
@@ -2669,7 +2716,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>302</v>
       </c>
@@ -2696,57 +2743,57 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2764,22 +2811,22 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>178</v>
       </c>

</xml_diff>